<commit_message>
working on NN and LSTM for floats
</commit_message>
<xml_diff>
--- a/opv_results.xlsx
+++ b/opv_results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Stanley Lo\Documents\Summer 2021 NSERC\ml_for_opvs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{780FE715-052D-49D8-9650-B7244C12809B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{956CB428-E5C9-485D-944A-658794626615}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" activeTab="5" xr2:uid="{89160D80-ECCB-4350-8EBA-80C0C1DD8511}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" activeTab="1" xr2:uid="{89160D80-ECCB-4350-8EBA-80C0C1DD8511}"/>
   </bookViews>
   <sheets>
     <sheet name="opv_results" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="471" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="480" uniqueCount="41">
   <si>
     <t>Summary of Model vs. Data Representation</t>
   </si>
@@ -432,6 +432,36 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-CA"/>
+              <a:t>R</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-CA" baseline="0"/>
+              <a:t> of PCE - RF Model</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-CA"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -916,7 +946,571 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>R of PCE - RF Model</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'for plotting'!$O$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>R</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:errBars>
+            <c:errBarType val="both"/>
+            <c:errValType val="cust"/>
+            <c:noEndCap val="0"/>
+            <c:plus>
+              <c:numRef>
+                <c:f>'for plotting'!$P$2:$P$6</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="5"/>
+                  <c:pt idx="0">
+                    <c:v>8.8524541626625403E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>8.3569494716285594E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>7.3440678332130804E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>0.209482533719349</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>0.207272858669764</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:plus>
+            <c:minus>
+              <c:numRef>
+                <c:f>'for plotting'!$P$2:$P$6</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="5"/>
+                  <c:pt idx="0">
+                    <c:v>8.8524541626625403E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>8.3569494716285594E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>7.3440678332130804E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>0.209482533719349</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>0.207272858669764</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:minus>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:errBars>
+          <c:cat>
+            <c:multiLvlStrRef>
+              <c:f>'for plotting'!$M$2:$N$6</c:f>
+              <c:multiLvlStrCache>
+                <c:ptCount val="5"/>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>Manual Fragments</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>Manual Fragments</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>Manual Fragments</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>Manual Fragments</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>Manual Fragments</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>error_corrected_data (n=567)</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>old data (n=386)</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>electronic (n=486)</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>device (n=80)</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>impt_device (n=108)</c:v>
+                  </c:pt>
+                </c:lvl>
+              </c:multiLvlStrCache>
+            </c:multiLvlStrRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'for plotting'!$O$2:$O$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>0.67665961088969695</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.51812458842905895</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.69799765338361097</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.38852529151653498</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.54144495253863301</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-0F9D-48C1-8A09-849EC020C3E1}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:dLblPos val="outEnd"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="834442832"/>
+        <c:axId val="834441584"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="834442832"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="834441584"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="834441584"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-CA"/>
+                  <a:t>R</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="834442832"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -1459,20 +2053,523 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>213360</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>7620</xdr:rowOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>45720</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>22860</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>365760</xdr:colOff>
-      <xdr:row>26</xdr:row>
-      <xdr:rowOff>30480</xdr:rowOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>266700</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>45720</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1492,6 +2589,42 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>167640</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>15240</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>426720</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3A5C5E12-840F-A1D1-0478-D6AF956A6793}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -1799,7 +2932,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A8006122-67A7-4469-ADD5-B623037ECCEC}">
   <dimension ref="A1:AV35"/>
   <sheetViews>
-    <sheetView topLeftCell="Z1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="AC24" sqref="AC24"/>
     </sheetView>
   </sheetViews>
@@ -3139,8 +4272,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3D475D60-FFAE-409E-8A1F-29BAE8738757}">
   <dimension ref="A1:AV35"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="AC24" sqref="AC24"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="T27" sqref="T27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7654,10 +8787,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DEDC4CFD-1BD9-4FF4-8437-2519E306281E}">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:P6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I36" sqref="I36"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="W6" sqref="W6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7665,7 +8798,7 @@
     <col min="1" max="1" width="25.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>37</v>
       </c>
@@ -7678,8 +8811,20 @@
       <c r="D1" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="M1" t="s">
+        <v>37</v>
+      </c>
+      <c r="N1" t="s">
+        <v>34</v>
+      </c>
+      <c r="O1" t="s">
+        <v>1</v>
+      </c>
+      <c r="P1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>36</v>
       </c>
@@ -7695,8 +8840,23 @@
         <f>opv_results_updated!AE3</f>
         <v>6.3964336543134298E-2</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="M2" t="s">
+        <v>36</v>
+      </c>
+      <c r="N2" t="str">
+        <f>opv_results_updated!V2</f>
+        <v>Manual Fragments</v>
+      </c>
+      <c r="O2">
+        <f>opv_results_updated!V3</f>
+        <v>0.67665961088969695</v>
+      </c>
+      <c r="P2">
+        <f>opv_results_updated!W3</f>
+        <v>8.8524541626625403E-2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>35</v>
       </c>
@@ -7712,8 +8872,23 @@
         <f>opv_results!AE3</f>
         <v>7.1580188319444293E-2</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="M3" t="s">
+        <v>35</v>
+      </c>
+      <c r="N3" t="str">
+        <f>opv_results!V2</f>
+        <v>Manual Fragments</v>
+      </c>
+      <c r="O3">
+        <f>opv_results!V3</f>
+        <v>0.51812458842905895</v>
+      </c>
+      <c r="P3">
+        <f>opv_results!W3</f>
+        <v>8.3569494716285594E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>38</v>
       </c>
@@ -7729,8 +8904,23 @@
         <f>electronic_opv_results!AE3</f>
         <v>4.24098231097974E-2</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="M4" t="s">
+        <v>38</v>
+      </c>
+      <c r="N4" t="str">
+        <f>electronic_opv_results!V2</f>
+        <v>Manual Fragments</v>
+      </c>
+      <c r="O4">
+        <f>electronic_opv_results!V3</f>
+        <v>0.69799765338361097</v>
+      </c>
+      <c r="P4">
+        <f>electronic_opv_results!W3</f>
+        <v>7.3440678332130804E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>39</v>
       </c>
@@ -7746,8 +8936,23 @@
         <f>device_opv_results!AE3</f>
         <v>0.27069625068716602</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="M5" t="s">
+        <v>39</v>
+      </c>
+      <c r="N5" t="str">
+        <f>device_opv_results!V2</f>
+        <v>Manual Fragments</v>
+      </c>
+      <c r="O5">
+        <f>device_opv_results!V3</f>
+        <v>0.38852529151653498</v>
+      </c>
+      <c r="P5">
+        <f>device_opv_results!W3</f>
+        <v>0.209482533719349</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>40</v>
       </c>
@@ -7762,6 +8967,21 @@
       <c r="D6">
         <f>impt_device_opv_results!AE3</f>
         <v>0.20463735715686601</v>
+      </c>
+      <c r="M6" t="s">
+        <v>40</v>
+      </c>
+      <c r="N6" t="str">
+        <f>impt_device_opv_results!V2</f>
+        <v>Manual Fragments</v>
+      </c>
+      <c r="O6">
+        <f>impt_device_opv_results!V3</f>
+        <v>0.54144495253863301</v>
+      </c>
+      <c r="P6">
+        <f>impt_device_opv_results!W3</f>
+        <v>0.207272858669764</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
working on data visualization
</commit_message>
<xml_diff>
--- a/opv_results.xlsx
+++ b/opv_results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Stanley Lo\Documents\Summer 2021 NSERC\ml_for_opvs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2663234-43FF-49D5-9B93-DBA186D52017}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53FB3125-8038-4704-9BA0-E6FF704A8D75}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3456" yWindow="3456" windowWidth="23040" windowHeight="12204" activeTab="1" xr2:uid="{89160D80-ECCB-4350-8EBA-80C0C1DD8511}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" firstSheet="1" activeTab="5" xr2:uid="{89160D80-ECCB-4350-8EBA-80C0C1DD8511}"/>
   </bookViews>
   <sheets>
     <sheet name="opv_results" sheetId="1" r:id="rId1"/>
@@ -19,6 +19,7 @@
     <sheet name="device_opv_results" sheetId="3" r:id="rId4"/>
     <sheet name="impt_device_opv_results" sheetId="4" r:id="rId5"/>
     <sheet name="for plotting" sheetId="6" r:id="rId6"/>
+    <sheet name="all_results" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="488" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="492" uniqueCount="51">
   <si>
     <t>Summary of Model vs. Data Representation</t>
   </si>
@@ -202,7 +203,28 @@
     <t>Min Group (n=567)</t>
   </si>
   <si>
-    <t>Saeki Group (n=567, incl. electronic)</t>
+    <t>Model</t>
+  </si>
+  <si>
+    <t>Datatype</t>
+  </si>
+  <si>
+    <t>Parameter</t>
+  </si>
+  <si>
+    <t>Saeki Group (n=567)</t>
+  </si>
+  <si>
+    <t>Fingerprints + Material Properties (HOMO, LUMO, Eg, Mw)</t>
+  </si>
+  <si>
+    <t>Saeki Group (n=566)</t>
+  </si>
+  <si>
+    <t>processing (n=108)</t>
+  </si>
+  <si>
+    <t>contact layer, mobilities --&gt; material properties</t>
   </si>
 </sst>
 </file>
@@ -531,6 +553,44 @@
             <a:effectLst/>
           </c:spPr>
           <c:invertIfNegative val="0"/>
+          <c:dPt>
+            <c:idx val="0"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000002-734F-47A8-B44F-D07351CB4477}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="1"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000001-734F-47A8-B44F-D07351CB4477}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
           <c:dLbls>
             <c:spPr>
               <a:noFill/>
@@ -595,23 +655,26 @@
             <c:noEndCap val="0"/>
             <c:plus>
               <c:numRef>
-                <c:f>'for plotting'!$D$4:$D$8</c:f>
+                <c:f>'for plotting'!$D$2:$D$8</c:f>
                 <c:numCache>
                   <c:formatCode>General</c:formatCode>
-                  <c:ptCount val="5"/>
-                  <c:pt idx="0">
+                  <c:ptCount val="7"/>
+                  <c:pt idx="1">
+                    <c:v>0.02</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
                     <c:v>6.3964336543134298E-2</c:v>
                   </c:pt>
-                  <c:pt idx="1">
+                  <c:pt idx="3">
                     <c:v>7.1580188319444293E-2</c:v>
                   </c:pt>
-                  <c:pt idx="2">
+                  <c:pt idx="4">
                     <c:v>4.24098231097974E-2</c:v>
                   </c:pt>
-                  <c:pt idx="3">
+                  <c:pt idx="5">
                     <c:v>0.27069625068716602</c:v>
                   </c:pt>
-                  <c:pt idx="4">
+                  <c:pt idx="6">
                     <c:v>0.20463735715686601</c:v>
                   </c:pt>
                 </c:numCache>
@@ -619,23 +682,26 @@
             </c:plus>
             <c:minus>
               <c:numRef>
-                <c:f>'for plotting'!$D$4:$D$8</c:f>
+                <c:f>'for plotting'!$D$2:$D$8</c:f>
                 <c:numCache>
                   <c:formatCode>General</c:formatCode>
-                  <c:ptCount val="5"/>
-                  <c:pt idx="0">
+                  <c:ptCount val="7"/>
+                  <c:pt idx="1">
+                    <c:v>0.02</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
                     <c:v>6.3964336543134298E-2</c:v>
                   </c:pt>
-                  <c:pt idx="1">
+                  <c:pt idx="3">
                     <c:v>7.1580188319444293E-2</c:v>
                   </c:pt>
-                  <c:pt idx="2">
+                  <c:pt idx="4">
                     <c:v>4.24098231097974E-2</c:v>
                   </c:pt>
-                  <c:pt idx="3">
+                  <c:pt idx="5">
                     <c:v>0.27069625068716602</c:v>
                   </c:pt>
-                  <c:pt idx="4">
+                  <c:pt idx="6">
                     <c:v>0.20463735715686601</c:v>
                   </c:pt>
                 </c:numCache>
@@ -657,15 +723,15 @@
           </c:errBars>
           <c:cat>
             <c:multiLvlStrRef>
-              <c:f>'for plotting'!$A$4:$B$8</c:f>
+              <c:f>'for plotting'!$A$2:$B$8</c:f>
               <c:multiLvlStrCache>
-                <c:ptCount val="5"/>
+                <c:ptCount val="7"/>
                 <c:lvl>
                   <c:pt idx="0">
-                    <c:v>Fingerprints</c:v>
+                    <c:v>Fragments</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>Fingerprints</c:v>
+                    <c:v>Fingerprints + Material Properties (HOMO, LUMO, Eg, Mw)</c:v>
                   </c:pt>
                   <c:pt idx="2">
                     <c:v>Fingerprints</c:v>
@@ -676,22 +742,34 @@
                   <c:pt idx="4">
                     <c:v>Fingerprints</c:v>
                   </c:pt>
+                  <c:pt idx="5">
+                    <c:v>Fingerprints</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>Fingerprints</c:v>
+                  </c:pt>
                 </c:lvl>
                 <c:lvl>
                   <c:pt idx="0">
+                    <c:v>Min Group (n=567)</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>Saeki Group (n=566)</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
                     <c:v>error_corrected_data (n=567)</c:v>
                   </c:pt>
-                  <c:pt idx="1">
+                  <c:pt idx="3">
                     <c:v>old data (n=386)</c:v>
                   </c:pt>
-                  <c:pt idx="2">
+                  <c:pt idx="4">
                     <c:v>electronic (n=486)</c:v>
                   </c:pt>
-                  <c:pt idx="3">
+                  <c:pt idx="5">
                     <c:v>device (n=80)</c:v>
                   </c:pt>
-                  <c:pt idx="4">
-                    <c:v>impt_device (n=108)</c:v>
+                  <c:pt idx="6">
+                    <c:v>processing (n=108)</c:v>
                   </c:pt>
                 </c:lvl>
               </c:multiLvlStrCache>
@@ -699,23 +777,29 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'for plotting'!$C$4:$C$8</c:f>
+              <c:f>'for plotting'!$C$2:$C$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
+                  <c:v>0.7</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.85</c:v>
+                </c:pt>
+                <c:pt idx="2">
                   <c:v>0.75023839873161102</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="3">
                   <c:v>0.63779712363765595</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="4">
                   <c:v>0.735927981000429</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="5">
                   <c:v>0.45407344336669903</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="6">
                   <c:v>0.49267380777903602</c:v>
                 </c:pt>
               </c:numCache>
@@ -2570,15 +2654,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>141276</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>76914</xdr:rowOff>
+      <xdr:colOff>147902</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>30530</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>470452</xdr:colOff>
-      <xdr:row>26</xdr:row>
-      <xdr:rowOff>96252</xdr:rowOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>563217</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>119269</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2605,16 +2689,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>192156</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>125894</xdr:rowOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>417443</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>46381</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>26</xdr:col>
-      <xdr:colOff>426719</xdr:colOff>
-      <xdr:row>30</xdr:row>
-      <xdr:rowOff>38099</xdr:rowOff>
+      <xdr:colOff>42406</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>144116</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -4281,8 +4365,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3D475D60-FFAE-409E-8A1F-29BAE8738757}">
   <dimension ref="A1:AV35"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="K13" sqref="K13"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="N26" sqref="N26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5476,7 +5560,7 @@
   <dimension ref="A1:AV35"/>
   <sheetViews>
     <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="L25" sqref="L25"/>
+      <selection activeCell="L63" sqref="L63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6610,7 +6694,7 @@
   <dimension ref="A1:AV35"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="K27" sqref="K27"/>
+      <selection activeCell="J18" sqref="J18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -8864,16 +8948,16 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DEDC4CFD-1BD9-4FF4-8437-2519E306281E}">
-  <dimension ref="A1:P8"/>
+  <dimension ref="A1:P9"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="J17" sqref="J17"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="25.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.77734375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="50" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.3">
@@ -8924,28 +9008,28 @@
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="B3" t="s">
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="C3">
         <v>0.85</v>
       </c>
       <c r="D3">
-        <v>0.01</v>
+        <v>0.02</v>
       </c>
       <c r="M3" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="N3" t="s">
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="O3">
         <v>0.85</v>
       </c>
       <c r="P3">
-        <v>0.01</v>
+        <v>0.02</v>
       </c>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.3">
@@ -9078,7 +9162,7 @@
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>40</v>
+        <v>49</v>
       </c>
       <c r="B8" t="str">
         <f>impt_device_opv_results!AD2</f>
@@ -9106,10 +9190,44 @@
       <c r="P8">
         <f>impt_device_opv_results!W3</f>
         <v>0.207272858669764</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>50</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A0E65A3-8569-483E-8B0E-AEAF20475785}">
+  <dimension ref="A1:C1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="3" max="3" width="9.5546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>